<commit_message>
Unit 9 recitation complete
Hospital OR optimization completed
</commit_message>
<xml_diff>
--- a/Unit 9 Integer Optimization/SportsScheduling.xlsx
+++ b/Unit 9 Integer Optimization/SportsScheduling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcampbell/Documents/GitHub/MIT-Analytics/Unit 9 Integer Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425373DE-6C89-CF4B-A5F5-A718BBB8BDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83675B5D-51A4-D440-B1D2-D0293E68DEF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="11520" windowHeight="13800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="13800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$14:$B$35</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$5:$G$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$36</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$37:$B$38</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$5:$G$8</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -30,14 +32,18 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$10</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">5</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$D$14:$D$35</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">binary</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$D$36</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$D$37:$D$38</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">binary</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="84">
   <si>
     <t>SPORTS SCHEDULING</t>
   </si>
@@ -188,13 +194,145 @@
   </si>
   <si>
     <t>D plays once in week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>AB twice</t>
+  </si>
+  <si>
+    <t>AC twice</t>
+  </si>
+  <si>
+    <t>BC twice</t>
+  </si>
+  <si>
+    <t>DE twice</t>
+  </si>
+  <si>
+    <t>DF twice</t>
+  </si>
+  <si>
+    <t>EF twice</t>
+  </si>
+  <si>
+    <t>AD once</t>
+  </si>
+  <si>
+    <t>AE once</t>
+  </si>
+  <si>
+    <t>AF once</t>
+  </si>
+  <si>
+    <t>BD once</t>
+  </si>
+  <si>
+    <t>BE once</t>
+  </si>
+  <si>
+    <t>BF once</t>
+  </si>
+  <si>
+    <t>CD once</t>
+  </si>
+  <si>
+    <t>CE once</t>
+  </si>
+  <si>
+    <t>CF once</t>
+  </si>
+  <si>
+    <t>A1-7</t>
+  </si>
+  <si>
+    <t>B1-7</t>
+  </si>
+  <si>
+    <t>C1-7</t>
+  </si>
+  <si>
+    <t>D1-7</t>
+  </si>
+  <si>
+    <t>E1-7</t>
+  </si>
+  <si>
+    <t>F1-7</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>AB not weeks 3 &amp; 4</t>
+  </si>
+  <si>
+    <t>If AB in 4, then 2</t>
+  </si>
+  <si>
+    <t>CD weeks 1 and 2</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,6 +344,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -260,11 +404,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -273,6 +428,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -612,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:Y38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,17 +779,17 @@
     <col min="1" max="1" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -652,8 +808,53 @@
       <c r="G4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>47</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" t="s">
+        <v>53</v>
+      </c>
+      <c r="V4" t="s">
+        <v>54</v>
+      </c>
+      <c r="W4" t="s">
+        <v>55</v>
+      </c>
+      <c r="X4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -675,16 +876,19 @@
       <c r="G5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D6" s="5">
         <v>0</v>
@@ -693,21 +897,24 @@
         <v>0</v>
       </c>
       <c r="F6" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
         <v>0</v>
@@ -716,13 +923,16 @@
         <v>0</v>
       </c>
       <c r="F7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -744,22 +954,38 @@
       <c r="G8" s="5">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3">
         <f>1*B5+2*B6+4*B7+8*B8+1*G5+2*G6+4*G7+8*G8</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>14</v>
       </c>
@@ -770,7 +996,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -785,7 +1011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -799,8 +1025,11 @@
       <c r="D15" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -814,8 +1043,11 @@
       <c r="D16" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -829,8 +1061,11 @@
       <c r="D17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -844,8 +1079,11 @@
       <c r="D18" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -859,8 +1097,11 @@
       <c r="D19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -874,8 +1115,11 @@
       <c r="D20" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -889,8 +1133,11 @@
       <c r="D21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -904,8 +1151,11 @@
       <c r="D22" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -919,8 +1169,11 @@
       <c r="D23" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -934,8 +1187,11 @@
       <c r="D24" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -949,8 +1205,11 @@
       <c r="D25" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -964,8 +1223,11 @@
       <c r="D26" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -979,8 +1241,11 @@
       <c r="D27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -994,8 +1259,11 @@
       <c r="D28" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1009,8 +1277,11 @@
       <c r="D29" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1024,8 +1295,11 @@
       <c r="D30" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1039,8 +1313,11 @@
       <c r="D31" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1054,8 +1331,11 @@
       <c r="D32" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1069,8 +1349,11 @@
       <c r="D33" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -1084,8 +1367,11 @@
       <c r="D34" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -1099,8 +1385,61 @@
       <c r="D35" s="4">
         <v>1</v>
       </c>
+      <c r="J35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="6">
+        <f>SUM(B7:B8)</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="6">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="6">
+        <f>B6</f>
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="6">
+        <f>B8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B38" s="6">
+        <f>SUM(G5:G6)</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>